<commit_message>
added conf upload+validate changed permissions of all files
</commit_message>
<xml_diff>
--- a/input_files/refs/demo1/Справочник компонентов потерь МСФО17.xlsx
+++ b/input_files/refs/demo1/Справочник компонентов потерь МСФО17.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bitoche\REPOS\USER\dissertation_project\input_files\refs\demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA16937-D201-4811-A212-7D67D6323F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1A949C-646A-48F8-B750-67BFC3FBCEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="17835" windowHeight="7635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -428,12 +428,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>